<commit_message>
Updated SA and hillclimbers
</commit_message>
<xml_diff>
--- a/Heuristieken_MM/main/Test.xlsx
+++ b/Heuristieken_MM/main/Test.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:AN33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,30 +449,115 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
           <t>amount of wires</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>directions of order</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>lower bound</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>netlist</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>order</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>upper bound</t>
         </is>
@@ -524,30 +609,81 @@
       <c r="O2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
       <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="n">
         <v>376</v>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T2" t="n">
+      <c r="AK2" t="n">
         <v>253</v>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W2" t="n">
+      <c r="AN2" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -594,31 +730,82 @@
       <c r="N3" t="n">
         <v>1</v>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
       <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="n">
         <v>376</v>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T3" t="n">
+      <c r="AK3" t="n">
         <v>253</v>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="AM3" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W3" t="n">
+      <c r="AN3" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -662,32 +849,83 @@
       <c r="M4" t="n">
         <v>2</v>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2</v>
+      </c>
       <c r="R4" t="n">
+        <v>2</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2</v>
+      </c>
+      <c r="T4" t="n">
+        <v>2</v>
+      </c>
+      <c r="U4" t="n">
+        <v>2</v>
+      </c>
+      <c r="V4" t="n">
+        <v>2</v>
+      </c>
+      <c r="W4" t="n">
+        <v>2</v>
+      </c>
+      <c r="X4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="n">
         <v>402</v>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="AJ4" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T4" t="n">
+      <c r="AK4" t="n">
         <v>253</v>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="AL4" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="AM4" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W4" t="n">
+      <c r="AN4" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -728,33 +966,84 @@
       <c r="L5" t="n">
         <v>3</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>3</v>
+      </c>
+      <c r="N5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O5" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>3</v>
+      </c>
       <c r="R5" t="n">
+        <v>3</v>
+      </c>
+      <c r="S5" t="n">
+        <v>3</v>
+      </c>
+      <c r="T5" t="n">
+        <v>3</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3</v>
+      </c>
+      <c r="V5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W5" t="n">
+        <v>3</v>
+      </c>
+      <c r="X5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="n">
         <v>387</v>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="AJ5" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T5" t="n">
+      <c r="AK5" t="n">
         <v>253</v>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="AL5" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="AM5" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W5" t="n">
+      <c r="AN5" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -792,34 +1081,85 @@
       <c r="K6" t="n">
         <v>4</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>4</v>
+      </c>
+      <c r="M6" t="n">
+        <v>4</v>
+      </c>
+      <c r="N6" t="n">
+        <v>4</v>
+      </c>
+      <c r="O6" t="n">
+        <v>4</v>
+      </c>
+      <c r="P6" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>4</v>
+      </c>
       <c r="R6" t="n">
+        <v>4</v>
+      </c>
+      <c r="S6" t="n">
+        <v>4</v>
+      </c>
+      <c r="T6" t="n">
+        <v>4</v>
+      </c>
+      <c r="U6" t="n">
+        <v>4</v>
+      </c>
+      <c r="V6" t="n">
+        <v>4</v>
+      </c>
+      <c r="W6" t="n">
+        <v>4</v>
+      </c>
+      <c r="X6" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="n">
         <v>402</v>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="AJ6" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T6" t="n">
+      <c r="AK6" t="n">
         <v>253</v>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="AL6" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V6" t="inlineStr">
+      <c r="AM6" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W6" t="n">
+      <c r="AN6" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -854,35 +1194,86 @@
       <c r="J7" t="n">
         <v>5</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>5</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>5</v>
+      </c>
+      <c r="O7" t="n">
+        <v>5</v>
+      </c>
+      <c r="P7" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>5</v>
+      </c>
       <c r="R7" t="n">
+        <v>5</v>
+      </c>
+      <c r="S7" t="n">
+        <v>5</v>
+      </c>
+      <c r="T7" t="n">
+        <v>5</v>
+      </c>
+      <c r="U7" t="n">
+        <v>5</v>
+      </c>
+      <c r="V7" t="n">
+        <v>5</v>
+      </c>
+      <c r="W7" t="n">
+        <v>5</v>
+      </c>
+      <c r="X7" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="n">
         <v>402</v>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="AJ7" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T7" t="n">
+      <c r="AK7" t="n">
         <v>253</v>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="AL7" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V7" t="inlineStr">
+      <c r="AM7" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W7" t="n">
+      <c r="AN7" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -914,36 +1305,87 @@
       <c r="I8" t="n">
         <v>6</v>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>6</v>
+      </c>
+      <c r="K8" t="n">
+        <v>6</v>
+      </c>
+      <c r="L8" t="n">
+        <v>6</v>
+      </c>
+      <c r="M8" t="n">
+        <v>6</v>
+      </c>
+      <c r="N8" t="n">
+        <v>6</v>
+      </c>
+      <c r="O8" t="n">
+        <v>6</v>
+      </c>
+      <c r="P8" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>6</v>
+      </c>
       <c r="R8" t="n">
+        <v>6</v>
+      </c>
+      <c r="S8" t="n">
+        <v>6</v>
+      </c>
+      <c r="T8" t="n">
+        <v>6</v>
+      </c>
+      <c r="U8" t="n">
+        <v>6</v>
+      </c>
+      <c r="V8" t="n">
+        <v>6</v>
+      </c>
+      <c r="W8" t="n">
+        <v>6</v>
+      </c>
+      <c r="X8" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="n">
         <v>348</v>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="AJ8" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T8" t="n">
+      <c r="AK8" t="n">
         <v>253</v>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="AL8" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V8" t="inlineStr">
+      <c r="AM8" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W8" t="n">
+      <c r="AN8" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -972,37 +1414,88 @@
       <c r="H9" t="n">
         <v>7</v>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>7</v>
+      </c>
+      <c r="J9" t="n">
+        <v>7</v>
+      </c>
+      <c r="K9" t="n">
+        <v>7</v>
+      </c>
+      <c r="L9" t="n">
+        <v>7</v>
+      </c>
+      <c r="M9" t="n">
+        <v>7</v>
+      </c>
+      <c r="N9" t="n">
+        <v>7</v>
+      </c>
+      <c r="O9" t="n">
+        <v>7</v>
+      </c>
+      <c r="P9" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>7</v>
+      </c>
       <c r="R9" t="n">
+        <v>7</v>
+      </c>
+      <c r="S9" t="n">
+        <v>7</v>
+      </c>
+      <c r="T9" t="n">
+        <v>7</v>
+      </c>
+      <c r="U9" t="n">
+        <v>7</v>
+      </c>
+      <c r="V9" t="n">
+        <v>7</v>
+      </c>
+      <c r="W9" t="n">
+        <v>7</v>
+      </c>
+      <c r="X9" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="n">
         <v>348</v>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="AJ9" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T9" t="n">
+      <c r="AK9" t="n">
         <v>253</v>
       </c>
-      <c r="U9" t="inlineStr">
+      <c r="AL9" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V9" t="inlineStr">
+      <c r="AM9" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W9" t="n">
+      <c r="AN9" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -1028,38 +1521,89 @@
       <c r="G10" t="n">
         <v>8</v>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>8</v>
+      </c>
+      <c r="I10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" t="n">
+        <v>8</v>
+      </c>
+      <c r="K10" t="n">
+        <v>8</v>
+      </c>
+      <c r="L10" t="n">
+        <v>8</v>
+      </c>
+      <c r="M10" t="n">
+        <v>8</v>
+      </c>
+      <c r="N10" t="n">
+        <v>8</v>
+      </c>
+      <c r="O10" t="n">
+        <v>8</v>
+      </c>
+      <c r="P10" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>8</v>
+      </c>
       <c r="R10" t="n">
+        <v>8</v>
+      </c>
+      <c r="S10" t="n">
+        <v>8</v>
+      </c>
+      <c r="T10" t="n">
+        <v>8</v>
+      </c>
+      <c r="U10" t="n">
+        <v>8</v>
+      </c>
+      <c r="V10" t="n">
+        <v>8</v>
+      </c>
+      <c r="W10" t="n">
+        <v>8</v>
+      </c>
+      <c r="X10" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="n">
         <v>348</v>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="AJ10" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T10" t="n">
+      <c r="AK10" t="n">
         <v>253</v>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="AL10" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V10" t="inlineStr">
+      <c r="AM10" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W10" t="n">
+      <c r="AN10" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -1082,39 +1626,90 @@
       <c r="F11" t="n">
         <v>9</v>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>9</v>
+      </c>
+      <c r="H11" t="n">
+        <v>9</v>
+      </c>
+      <c r="I11" t="n">
+        <v>9</v>
+      </c>
+      <c r="J11" t="n">
+        <v>9</v>
+      </c>
+      <c r="K11" t="n">
+        <v>9</v>
+      </c>
+      <c r="L11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M11" t="n">
+        <v>9</v>
+      </c>
+      <c r="N11" t="n">
+        <v>9</v>
+      </c>
+      <c r="O11" t="n">
+        <v>9</v>
+      </c>
+      <c r="P11" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>9</v>
+      </c>
       <c r="R11" t="n">
+        <v>9</v>
+      </c>
+      <c r="S11" t="n">
+        <v>9</v>
+      </c>
+      <c r="T11" t="n">
+        <v>9</v>
+      </c>
+      <c r="U11" t="n">
+        <v>9</v>
+      </c>
+      <c r="V11" t="n">
+        <v>9</v>
+      </c>
+      <c r="W11" t="n">
+        <v>9</v>
+      </c>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="n">
         <v>402</v>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="AJ11" t="inlineStr">
         <is>
           <t>['diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical', 'vertical']</t>
         </is>
       </c>
-      <c r="T11" t="n">
+      <c r="AK11" t="n">
         <v>253</v>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="AL11" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V11" t="inlineStr">
+      <c r="AM11" t="inlineStr">
         <is>
           <t>[(14, 12), (18, 12), (11, 21), (15, 8), (15, 6), (25, 13), (9, 24), (15, 2), (3, 6), (12, 13), (17, 22), (19, 22), (16, 14), (5, 4), (4, 1), (7, 10), (20, 10), (13, 21), (24, 21), (12, 8), (11, 5), (10, 24), (16, 5), (1, 16), (6, 18), (2, 23), (2, 22)]</t>
         </is>
       </c>
-      <c r="W11" t="n">
+      <c r="AN11" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -1134,40 +1729,91 @@
       <c r="E12" t="n">
         <v>10</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
+      <c r="I12" t="n">
+        <v>10</v>
+      </c>
+      <c r="J12" t="n">
+        <v>10</v>
+      </c>
+      <c r="K12" t="n">
+        <v>10</v>
+      </c>
+      <c r="L12" t="n">
+        <v>10</v>
+      </c>
+      <c r="M12" t="n">
+        <v>10</v>
+      </c>
+      <c r="N12" t="n">
+        <v>10</v>
+      </c>
+      <c r="O12" t="n">
+        <v>10</v>
+      </c>
+      <c r="P12" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>10</v>
+      </c>
       <c r="R12" t="n">
+        <v>10</v>
+      </c>
+      <c r="S12" t="n">
+        <v>10</v>
+      </c>
+      <c r="T12" t="n">
+        <v>10</v>
+      </c>
+      <c r="U12" t="n">
+        <v>10</v>
+      </c>
+      <c r="V12" t="n">
+        <v>10</v>
+      </c>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="n">
         <v>348</v>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="AJ12" t="inlineStr">
         <is>
           <t>['diagonal', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'vertical', 'horizontal', 'horizontal', 'vertical', 'horizontal']</t>
         </is>
       </c>
-      <c r="T12" t="n">
+      <c r="AK12" t="n">
         <v>243</v>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="AL12" t="inlineStr">
         <is>
           <t>netlist_2</t>
         </is>
       </c>
-      <c r="V12" t="inlineStr">
+      <c r="AM12" t="inlineStr">
         <is>
           <t>[(21, 11), (6, 8), (23, 17), (4, 16), (11, 8), (11, 5), (17, 10), (10, 14), (20, 3), (24, 9), (8, 10), (20, 6), (3, 21), (16, 22), (4, 24), (16, 18), (16, 6), (14, 19), (16, 9), (8, 14), (7, 15), (21, 20), (2, 1), (24, 5), (4, 6)]</t>
         </is>
       </c>
-      <c r="W12" t="n">
+      <c r="AN12" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -1184,41 +1830,92 @@
       <c r="D13" t="n">
         <v>11</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>11</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" t="n">
+        <v>11</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11</v>
+      </c>
+      <c r="I13" t="n">
+        <v>11</v>
+      </c>
+      <c r="J13" t="n">
+        <v>11</v>
+      </c>
+      <c r="K13" t="n">
+        <v>11</v>
+      </c>
+      <c r="L13" t="n">
+        <v>11</v>
+      </c>
+      <c r="M13" t="n">
+        <v>11</v>
+      </c>
+      <c r="N13" t="n">
+        <v>11</v>
+      </c>
+      <c r="O13" t="n">
+        <v>11</v>
+      </c>
+      <c r="P13" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>11</v>
+      </c>
       <c r="R13" t="n">
+        <v>11</v>
+      </c>
+      <c r="S13" t="n">
+        <v>11</v>
+      </c>
+      <c r="T13" t="n">
+        <v>11</v>
+      </c>
+      <c r="U13" t="n">
+        <v>11</v>
+      </c>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="n">
         <v>537</v>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="AJ13" t="inlineStr">
         <is>
           <t>['horizontal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'diagonal', 'vertical', 'horizontal', 'vertical', 'horizontal', 'horizontal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal']</t>
         </is>
       </c>
-      <c r="T13" t="n">
+      <c r="AK13" t="n">
         <v>311</v>
       </c>
-      <c r="U13" t="inlineStr">
+      <c r="AL13" t="inlineStr">
         <is>
           <t>netlist_3</t>
         </is>
       </c>
-      <c r="V13" t="inlineStr">
+      <c r="AM13" t="inlineStr">
         <is>
           <t>[(18, 16), (1, 23), (16, 22), (13, 25), (25, 16), (3, 17), (2, 14), (12, 4), (9, 10), (6, 13), (11, 2), (25, 17), (23, 19), (6, 15), (23, 12), (8, 6), (8, 24), (12, 1), (19, 11), (17, 8), (19, 3), (5, 2), (14, 3), (21, 7), (3, 4), (12, 18), (21, 17), (14, 20), (19, 21), (1, 15), (4, 10), (20, 22)]</t>
         </is>
       </c>
-      <c r="W13" t="n">
+      <c r="AN13" t="n">
         <v>10584</v>
       </c>
     </row>
@@ -1232,42 +1929,93 @@
       <c r="C14" t="n">
         <v>12</v>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="n">
+        <v>12</v>
+      </c>
+      <c r="F14" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>12</v>
+      </c>
+      <c r="H14" t="n">
+        <v>12</v>
+      </c>
+      <c r="I14" t="n">
+        <v>12</v>
+      </c>
+      <c r="J14" t="n">
+        <v>12</v>
+      </c>
+      <c r="K14" t="n">
+        <v>12</v>
+      </c>
+      <c r="L14" t="n">
+        <v>12</v>
+      </c>
+      <c r="M14" t="n">
+        <v>12</v>
+      </c>
+      <c r="N14" t="n">
+        <v>12</v>
+      </c>
+      <c r="O14" t="n">
+        <v>12</v>
+      </c>
+      <c r="P14" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>12</v>
+      </c>
       <c r="R14" t="n">
+        <v>12</v>
+      </c>
+      <c r="S14" t="n">
+        <v>12</v>
+      </c>
+      <c r="T14" t="n">
+        <v>12</v>
+      </c>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="n">
         <v>714</v>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="AJ14" t="inlineStr">
         <is>
           <t>['horizontal', 'horizontal', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'vertical', 'horizontal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'horizontal', 'vertical', 'horizontal', 'horizontal', 'diagonal', 'vertical']</t>
         </is>
       </c>
-      <c r="T14" t="n">
+      <c r="AK14" t="n">
         <v>437</v>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="AL14" t="inlineStr">
         <is>
           <t>netlist_4</t>
         </is>
       </c>
-      <c r="V14" t="inlineStr">
+      <c r="AM14" t="inlineStr">
         <is>
           <t>[(22, 8), (47, 36), (36, 20), (44, 31), (5, 30), (1, 22), (32, 26), (33, 30), (29, 44), (23, 50), (15, 40), (5, 24), (18, 26), (42, 2), (40, 16), (37, 3), (13, 2), (29, 28), (21, 41), (6, 45), (15, 5), (5, 31), (40, 19), (37, 5), (4, 32), (4, 49), (50, 14), (15, 7), (30, 10), (34, 31), (47, 1), (1, 13), (3, 4), (35, 46), (44, 16)]</t>
         </is>
       </c>
-      <c r="W14" t="n">
+      <c r="AN14" t="n">
         <v>14112</v>
       </c>
     </row>
@@ -1278,43 +2026,94 @@
       <c r="B15" t="n">
         <v>13</v>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13</v>
+      </c>
+      <c r="F15" t="n">
+        <v>13</v>
+      </c>
+      <c r="G15" t="n">
+        <v>13</v>
+      </c>
+      <c r="H15" t="n">
+        <v>13</v>
+      </c>
+      <c r="I15" t="n">
+        <v>13</v>
+      </c>
+      <c r="J15" t="n">
+        <v>13</v>
+      </c>
+      <c r="K15" t="n">
+        <v>13</v>
+      </c>
+      <c r="L15" t="n">
+        <v>13</v>
+      </c>
+      <c r="M15" t="n">
+        <v>13</v>
+      </c>
+      <c r="N15" t="n">
+        <v>13</v>
+      </c>
+      <c r="O15" t="n">
+        <v>13</v>
+      </c>
+      <c r="P15" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>13</v>
+      </c>
       <c r="R15" t="n">
+        <v>13</v>
+      </c>
+      <c r="S15" t="n">
+        <v>13</v>
+      </c>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="n">
         <v>543</v>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="AJ15" t="inlineStr">
         <is>
           <t>['horizontal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'vertical', 'horizontal', 'vertical', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'diagonal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'vertical', 'diagonal', 'vertical', 'diagonal', 'vertical']</t>
         </is>
       </c>
-      <c r="T15" t="n">
+      <c r="AK15" t="n">
         <v>366</v>
       </c>
-      <c r="U15" t="inlineStr">
+      <c r="AL15" t="inlineStr">
         <is>
           <t>netlist_4</t>
         </is>
       </c>
-      <c r="V15" t="inlineStr">
+      <c r="AM15" t="inlineStr">
         <is>
           <t>[(5, 9), (26, 50), (13, 26), (33, 12), (10, 6), (49, 48), (34, 5), (34, 37), (36, 7), (35, 6), (42, 14), (16, 43), (20, 34), (1, 17), (21, 48), (28, 23), (48, 6), (1, 22), (3, 18), (40, 49), (44, 45), (26, 25), (45, 35), (14, 50), (46, 19), (19, 12), (41, 11), (2, 4), (45, 30), (21, 30), (5, 41), (8, 29), (27, 2), (13, 25), (18, 4)]</t>
         </is>
       </c>
-      <c r="W15" t="n">
+      <c r="AN15" t="n">
         <v>14112</v>
       </c>
     </row>
@@ -1322,44 +2121,1421 @@
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" t="n">
+        <v>14</v>
+      </c>
+      <c r="F16" t="n">
+        <v>14</v>
+      </c>
+      <c r="G16" t="n">
+        <v>14</v>
+      </c>
+      <c r="H16" t="n">
+        <v>14</v>
+      </c>
+      <c r="I16" t="n">
+        <v>14</v>
+      </c>
+      <c r="J16" t="n">
+        <v>14</v>
+      </c>
+      <c r="K16" t="n">
+        <v>14</v>
+      </c>
+      <c r="L16" t="n">
+        <v>14</v>
+      </c>
+      <c r="M16" t="n">
+        <v>14</v>
+      </c>
+      <c r="N16" t="n">
+        <v>14</v>
+      </c>
+      <c r="O16" t="n">
+        <v>14</v>
+      </c>
+      <c r="P16" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>14</v>
+      </c>
       <c r="R16" t="n">
+        <v>14</v>
+      </c>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="n">
         <v>796</v>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="AJ16" t="inlineStr">
         <is>
           <t>['diagonal', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'horizontal', 'horizontal', 'diagonal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'vertical', 'horizontal', 'vertical', 'vertical', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'horizontal']</t>
         </is>
       </c>
-      <c r="T16" t="n">
+      <c r="AK16" t="n">
         <v>472</v>
       </c>
-      <c r="U16" t="inlineStr">
+      <c r="AL16" t="inlineStr">
         <is>
           <t>netlist_6</t>
         </is>
       </c>
-      <c r="V16" t="inlineStr">
+      <c r="AM16" t="inlineStr">
         <is>
           <t>[(39, 8), (33, 26), (44, 32), (23, 45), (31, 33), (7, 34), (34, 32), (34, 8), (40, 39), (18, 36), (41, 48), (45, 35), (19, 43), (38, 3), (22, 43), (1, 4), (15, 35), (22, 34), (49, 3), (49, 35), (27, 40), (2, 38), (38, 44), (31, 41), (40, 4), (30, 38), (9, 5), (26, 7), (2, 14), (4, 11), (6, 40), (50, 13), (17, 9), (1, 40), (27, 42), (13, 6), (31, 8), (14, 46), (47, 1), (38, 41)]</t>
         </is>
       </c>
-      <c r="W16" t="n">
+      <c r="AN16" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G17" t="n">
+        <v>15</v>
+      </c>
+      <c r="H17" t="n">
+        <v>15</v>
+      </c>
+      <c r="I17" t="n">
+        <v>15</v>
+      </c>
+      <c r="J17" t="n">
+        <v>15</v>
+      </c>
+      <c r="K17" t="n">
+        <v>15</v>
+      </c>
+      <c r="L17" t="n">
+        <v>15</v>
+      </c>
+      <c r="M17" t="n">
+        <v>15</v>
+      </c>
+      <c r="N17" t="n">
+        <v>15</v>
+      </c>
+      <c r="O17" t="n">
+        <v>15</v>
+      </c>
+      <c r="P17" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>15</v>
+      </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="n">
+        <v>390</v>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>['horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'vertical', 'diagonal', 'vertical', 'vertical', 'horizontal', 'horizontal']</t>
+        </is>
+      </c>
+      <c r="AK17" t="n">
+        <v>253</v>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>netlist_2</t>
+        </is>
+      </c>
+      <c r="AM17" t="inlineStr">
+        <is>
+          <t>[(17, 22), (12, 13), (19, 22), (12, 8), (24, 21), (9, 24), (14, 12), (6, 18), (15, 6), (3, 6), (11, 21), (25, 13), (11, 5), (4, 1), (15, 2), (15, 8), (16, 14), (7, 10), (13, 21), (2, 23), (1, 16), (2, 22), (18, 12), (16, 5), (10, 24), (20, 10), (5, 4)]</t>
+        </is>
+      </c>
+      <c r="AN17" t="n">
+        <v>10584</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="n">
+        <v>16</v>
+      </c>
+      <c r="F18" t="n">
+        <v>16</v>
+      </c>
+      <c r="G18" t="n">
+        <v>16</v>
+      </c>
+      <c r="H18" t="n">
+        <v>16</v>
+      </c>
+      <c r="I18" t="n">
+        <v>16</v>
+      </c>
+      <c r="J18" t="n">
+        <v>16</v>
+      </c>
+      <c r="K18" t="n">
+        <v>16</v>
+      </c>
+      <c r="L18" t="n">
+        <v>16</v>
+      </c>
+      <c r="M18" t="n">
+        <v>16</v>
+      </c>
+      <c r="N18" t="n">
+        <v>16</v>
+      </c>
+      <c r="O18" t="n">
+        <v>16</v>
+      </c>
+      <c r="P18" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr"/>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="n">
+        <v>370</v>
+      </c>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>['horizontal', 'horizontal', 'diagonal', 'vertical', 'vertical', 'vertical', 'vertical', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'vertical']</t>
+        </is>
+      </c>
+      <c r="AK18" t="n">
+        <v>253</v>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>netlist_2</t>
+        </is>
+      </c>
+      <c r="AM18" t="inlineStr">
+        <is>
+          <t>[(17, 22), (4, 1), (25, 13), (6, 18), (2, 22), (1, 16), (12, 8), (3, 6), (14, 12), (12, 13), (15, 6), (2, 23), (16, 14), (20, 10), (15, 2), (7, 10), (15, 8), (5, 4), (10, 24), (13, 21), (11, 21), (11, 5), (9, 24), (19, 22), (16, 5), (18, 12), (24, 21)]</t>
+        </is>
+      </c>
+      <c r="AN18" t="n">
+        <v>10584</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" t="n">
+        <v>17</v>
+      </c>
+      <c r="F19" t="n">
+        <v>17</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17</v>
+      </c>
+      <c r="H19" t="n">
+        <v>17</v>
+      </c>
+      <c r="I19" t="n">
+        <v>17</v>
+      </c>
+      <c r="J19" t="n">
+        <v>17</v>
+      </c>
+      <c r="K19" t="n">
+        <v>17</v>
+      </c>
+      <c r="L19" t="n">
+        <v>17</v>
+      </c>
+      <c r="M19" t="n">
+        <v>17</v>
+      </c>
+      <c r="N19" t="n">
+        <v>17</v>
+      </c>
+      <c r="O19" t="n">
+        <v>17</v>
+      </c>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="n">
+        <v>376</v>
+      </c>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>['horizontal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'vertical', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'vertical']</t>
+        </is>
+      </c>
+      <c r="AK19" t="n">
+        <v>253</v>
+      </c>
+      <c r="AL19" t="inlineStr">
+        <is>
+          <t>netlist_2</t>
+        </is>
+      </c>
+      <c r="AM19" t="inlineStr">
+        <is>
+          <t>[(13, 21), (6, 18), (20, 10), (14, 12), (16, 5), (11, 5), (15, 2), (24, 21), (9, 24), (18, 12), (11, 21), (19, 22), (2, 23), (10, 24), (15, 8), (25, 13), (16, 14), (17, 22), (5, 4), (4, 1), (12, 13), (3, 6), (12, 8), (7, 10), (15, 6), (1, 16), (2, 22)]</t>
+        </is>
+      </c>
+      <c r="AN19" t="n">
+        <v>10584</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" t="n">
+        <v>18</v>
+      </c>
+      <c r="F20" t="n">
+        <v>18</v>
+      </c>
+      <c r="G20" t="n">
+        <v>18</v>
+      </c>
+      <c r="H20" t="n">
+        <v>18</v>
+      </c>
+      <c r="I20" t="n">
+        <v>18</v>
+      </c>
+      <c r="J20" t="n">
+        <v>18</v>
+      </c>
+      <c r="K20" t="n">
+        <v>18</v>
+      </c>
+      <c r="L20" t="n">
+        <v>18</v>
+      </c>
+      <c r="M20" t="n">
+        <v>18</v>
+      </c>
+      <c r="N20" t="n">
+        <v>18</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
+      <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="n">
+        <v>567</v>
+      </c>
+      <c r="AJ20" t="inlineStr">
+        <is>
+          <t>['horizontal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'diagonal', 'vertical', 'vertical', 'horizontal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'vertical', 'horizontal', 'vertical', 'vertical', 'vertical']</t>
+        </is>
+      </c>
+      <c r="AK20" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM20" t="inlineStr">
+        <is>
+          <t>[(5, 9), (34, 37), (42, 14), (33, 12), (21, 48), (34, 5), (48, 6), (16, 43), (26, 25), (5, 41), (2, 4), (45, 30), (13, 26), (36, 7), (20, 34), (14, 50), (13, 25), (1, 22), (45, 35), (41, 11), (18, 4), (35, 6), (49, 48), (28, 23), (10, 6), (46, 19), (8, 29), (40, 49), (3, 18), (44, 45), (26, 50), (1, 17), (27, 2), (19, 12), (21, 30)]</t>
+        </is>
+      </c>
+      <c r="AN20" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>19</v>
+      </c>
+      <c r="E21" t="n">
+        <v>19</v>
+      </c>
+      <c r="F21" t="n">
+        <v>19</v>
+      </c>
+      <c r="G21" t="n">
+        <v>19</v>
+      </c>
+      <c r="H21" t="n">
+        <v>19</v>
+      </c>
+      <c r="I21" t="n">
+        <v>19</v>
+      </c>
+      <c r="J21" t="n">
+        <v>19</v>
+      </c>
+      <c r="K21" t="n">
+        <v>19</v>
+      </c>
+      <c r="L21" t="n">
+        <v>19</v>
+      </c>
+      <c r="M21" t="n">
+        <v>19</v>
+      </c>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="n">
+        <v>533</v>
+      </c>
+      <c r="AJ21" t="inlineStr">
+        <is>
+          <t>['diagonal', 'horizontal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'vertical', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'horizontal']</t>
+        </is>
+      </c>
+      <c r="AK21" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL21" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM21" t="inlineStr">
+        <is>
+          <t>[(13, 25), (34, 37), (21, 48), (36, 7), (5, 9), (19, 12), (21, 30), (26, 25), (26, 50), (28, 23), (34, 5), (46, 19), (44, 45), (45, 35), (13, 26), (27, 2), (48, 6), (40, 49), (2, 4), (42, 14), (18, 4), (8, 29), (35, 6), (1, 17), (33, 12), (5, 41), (41, 11), (10, 6), (3, 18), (16, 43), (49, 48), (45, 30), (14, 50), (20, 34), (1, 22)]</t>
+        </is>
+      </c>
+      <c r="AN21" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" t="n">
+        <v>20</v>
+      </c>
+      <c r="F22" t="n">
+        <v>20</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" t="n">
+        <v>20</v>
+      </c>
+      <c r="I22" t="n">
+        <v>20</v>
+      </c>
+      <c r="J22" t="n">
+        <v>20</v>
+      </c>
+      <c r="K22" t="n">
+        <v>20</v>
+      </c>
+      <c r="L22" t="n">
+        <v>20</v>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr"/>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="n">
+        <v>495</v>
+      </c>
+      <c r="AJ22" t="inlineStr">
+        <is>
+          <t>['horizontal', 'vertical', 'diagonal', 'vertical', 'vertical', 'vertical', 'vertical', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'diagonal', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'horizontal', 'vertical', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'horizontal', 'diagonal']</t>
+        </is>
+      </c>
+      <c r="AK22" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL22" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM22" t="inlineStr">
+        <is>
+          <t>[(44, 45), (27, 2), (42, 14), (48, 6), (18, 4), (10, 6), (5, 41), (41, 11), (21, 48), (1, 22), (1, 17), (33, 12), (3, 18), (16, 43), (35, 6), (14, 50), (28, 23), (34, 5), (21, 30), (13, 25), (26, 25), (49, 48), (5, 9), (2, 4), (46, 19), (13, 26), (26, 50), (40, 49), (20, 34), (36, 7), (45, 35), (45, 30), (19, 12), (34, 37), (8, 29)]</t>
+        </is>
+      </c>
+      <c r="AN22" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
+      </c>
+      <c r="E23" t="n">
+        <v>21</v>
+      </c>
+      <c r="F23" t="n">
+        <v>21</v>
+      </c>
+      <c r="G23" t="n">
+        <v>21</v>
+      </c>
+      <c r="H23" t="n">
+        <v>21</v>
+      </c>
+      <c r="I23" t="n">
+        <v>21</v>
+      </c>
+      <c r="J23" t="n">
+        <v>21</v>
+      </c>
+      <c r="K23" t="n">
+        <v>21</v>
+      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="n">
+        <v>547</v>
+      </c>
+      <c r="AJ23" t="inlineStr">
+        <is>
+          <t>['diagonal', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'horizontal', 'vertical', 'vertical', 'horizontal', 'vertical', 'vertical', 'diagonal', 'vertical', 'vertical', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'horizontal']</t>
+        </is>
+      </c>
+      <c r="AK23" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL23" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM23" t="inlineStr">
+        <is>
+          <t>[(40, 49), (2, 4), (41, 11), (16, 43), (1, 17), (34, 5), (26, 25), (14, 50), (36, 7), (44, 45), (3, 18), (49, 48), (33, 12), (19, 12), (34, 37), (35, 6), (20, 34), (1, 22), (46, 19), (27, 2), (8, 29), (18, 4), (48, 6), (13, 26), (21, 48), (10, 6), (26, 50), (5, 41), (42, 14), (45, 35), (45, 30), (21, 30), (13, 25), (28, 23), (5, 9)]</t>
+        </is>
+      </c>
+      <c r="AN23" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>22</v>
+      </c>
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>22</v>
+      </c>
+      <c r="E24" t="n">
+        <v>22</v>
+      </c>
+      <c r="F24" t="n">
+        <v>22</v>
+      </c>
+      <c r="G24" t="n">
+        <v>22</v>
+      </c>
+      <c r="H24" t="n">
+        <v>22</v>
+      </c>
+      <c r="I24" t="n">
+        <v>22</v>
+      </c>
+      <c r="J24" t="n">
+        <v>22</v>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr"/>
+      <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="inlineStr"/>
+      <c r="AE24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="inlineStr"/>
+      <c r="AI24" t="n">
+        <v>539</v>
+      </c>
+      <c r="AJ24" t="inlineStr">
+        <is>
+          <t>['horizontal', 'diagonal', 'horizontal', 'vertical', 'vertical', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'horizontal', 'horizontal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'vertical', 'horizontal', 'horizontal', 'vertical', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'diagonal', 'diagonal', 'vertical']</t>
+        </is>
+      </c>
+      <c r="AK24" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL24" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM24" t="inlineStr">
+        <is>
+          <t>[(13, 26), (8, 29), (1, 22), (10, 6), (21, 30), (1, 17), (48, 6), (28, 23), (40, 49), (45, 35), (34, 37), (20, 34), (45, 30), (2, 4), (16, 43), (36, 7), (19, 12), (26, 50), (44, 45), (49, 48), (21, 48), (18, 4), (26, 25), (14, 50), (3, 18), (41, 11), (35, 6), (13, 25), (5, 9), (5, 41), (46, 19), (34, 5), (33, 12), (42, 14), (27, 2)]</t>
+        </is>
+      </c>
+      <c r="AN24" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>23</v>
+      </c>
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" t="n">
+        <v>23</v>
+      </c>
+      <c r="F25" t="n">
+        <v>23</v>
+      </c>
+      <c r="G25" t="n">
+        <v>23</v>
+      </c>
+      <c r="H25" t="n">
+        <v>23</v>
+      </c>
+      <c r="I25" t="n">
+        <v>23</v>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr"/>
+      <c r="AC25" t="inlineStr"/>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr"/>
+      <c r="AH25" t="inlineStr"/>
+      <c r="AI25" t="n">
+        <v>539</v>
+      </c>
+      <c r="AJ25" t="inlineStr">
+        <is>
+          <t>['diagonal', 'vertical', 'horizontal', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'horizontal', 'vertical', 'horizontal', 'vertical', 'diagonal', 'vertical', 'diagonal', 'vertical', 'diagonal', 'vertical', 'vertical', 'diagonal', 'vertical', 'horizontal', 'diagonal']</t>
+        </is>
+      </c>
+      <c r="AK25" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL25" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM25" t="inlineStr">
+        <is>
+          <t>[(40, 49), (10, 6), (28, 23), (13, 25), (44, 45), (5, 41), (41, 11), (1, 17), (26, 50), (5, 9), (3, 18), (42, 14), (49, 48), (36, 7), (14, 50), (13, 26), (26, 25), (45, 35), (19, 12), (27, 2), (1, 22), (48, 6), (34, 37), (46, 19), (45, 30), (20, 34), (8, 29), (18, 4), (16, 43), (35, 6), (21, 48), (34, 5), (21, 30), (2, 4), (33, 12)]</t>
+        </is>
+      </c>
+      <c r="AN25" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>24</v>
+      </c>
+      <c r="C26" t="n">
+        <v>24</v>
+      </c>
+      <c r="D26" t="n">
+        <v>24</v>
+      </c>
+      <c r="E26" t="n">
+        <v>24</v>
+      </c>
+      <c r="F26" t="n">
+        <v>24</v>
+      </c>
+      <c r="G26" t="n">
+        <v>24</v>
+      </c>
+      <c r="H26" t="n">
+        <v>24</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr"/>
+      <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="n">
+        <v>525</v>
+      </c>
+      <c r="AJ26" t="inlineStr">
+        <is>
+          <t>['horizontal', 'vertical', 'vertical', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'vertical', 'vertical']</t>
+        </is>
+      </c>
+      <c r="AK26" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL26" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM26" t="inlineStr">
+        <is>
+          <t>[(45, 35), (21, 48), (21, 30), (16, 43), (5, 41), (8, 29), (13, 26), (48, 6), (33, 12), (2, 4), (26, 25), (28, 23), (19, 12), (1, 17), (42, 14), (14, 50), (5, 9), (3, 18), (45, 30), (10, 6), (34, 5), (36, 7), (35, 6), (1, 22), (49, 48), (46, 19), (27, 2), (41, 11), (34, 37), (44, 45), (13, 25), (20, 34), (40, 49), (26, 50), (18, 4)]</t>
+        </is>
+      </c>
+      <c r="AN26" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>25</v>
+      </c>
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>25</v>
+      </c>
+      <c r="E27" t="n">
+        <v>25</v>
+      </c>
+      <c r="F27" t="n">
+        <v>25</v>
+      </c>
+      <c r="G27" t="n">
+        <v>25</v>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
+      <c r="AI27" t="n">
+        <v>521</v>
+      </c>
+      <c r="AJ27" t="inlineStr">
+        <is>
+          <t>['horizontal', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'vertical', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'vertical', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'vertical', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'vertical', 'horizontal', 'vertical']</t>
+        </is>
+      </c>
+      <c r="AK27" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL27" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM27" t="inlineStr">
+        <is>
+          <t>[(26, 25), (40, 49), (44, 45), (27, 2), (33, 12), (20, 34), (5, 9), (5, 41), (45, 35), (3, 18), (41, 11), (35, 6), (1, 22), (16, 43), (46, 19), (19, 12), (26, 50), (49, 48), (36, 7), (42, 14), (10, 6), (34, 37), (13, 25), (45, 30), (1, 17), (14, 50), (48, 6), (18, 4), (34, 5), (8, 29), (28, 23), (2, 4), (21, 48), (13, 26), (21, 30)]</t>
+        </is>
+      </c>
+      <c r="AN27" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>26</v>
+      </c>
+      <c r="C28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D28" t="n">
+        <v>26</v>
+      </c>
+      <c r="E28" t="n">
+        <v>26</v>
+      </c>
+      <c r="F28" t="n">
+        <v>26</v>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
+      <c r="AI28" t="n">
+        <v>509</v>
+      </c>
+      <c r="AJ28" t="inlineStr">
+        <is>
+          <t>['vertical', 'vertical', 'vertical', 'vertical', 'diagonal', 'horizontal', 'vertical', 'vertical', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal']</t>
+        </is>
+      </c>
+      <c r="AK28" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL28" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM28" t="inlineStr">
+        <is>
+          <t>[(48, 6), (21, 48), (27, 2), (21, 30), (16, 43), (2, 4), (5, 41), (18, 4), (26, 50), (14, 50), (5, 9), (3, 18), (1, 17), (45, 30), (10, 6), (33, 12), (8, 29), (45, 35), (36, 7), (34, 5), (40, 49), (41, 11), (20, 34), (1, 22), (13, 26), (46, 19), (35, 6), (13, 25), (44, 45), (19, 12), (42, 14), (28, 23), (26, 25), (34, 37), (49, 48)]</t>
+        </is>
+      </c>
+      <c r="AN28" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>27</v>
+      </c>
+      <c r="C29" t="n">
+        <v>27</v>
+      </c>
+      <c r="D29" t="n">
+        <v>27</v>
+      </c>
+      <c r="E29" t="n">
+        <v>27</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
+      <c r="AI29" t="n">
+        <v>489</v>
+      </c>
+      <c r="AJ29" t="inlineStr">
+        <is>
+          <t>['diagonal', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'diagonal', 'diagonal', 'vertical', 'vertical', 'vertical', 'horizontal', 'vertical', 'vertical', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'diagonal']</t>
+        </is>
+      </c>
+      <c r="AK29" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL29" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM29" t="inlineStr">
+        <is>
+          <t>[(16, 43), (36, 7), (46, 19), (26, 25), (49, 48), (28, 23), (26, 50), (48, 6), (14, 50), (1, 22), (44, 45), (5, 9), (45, 35), (35, 6), (8, 29), (34, 5), (5, 41), (21, 30), (10, 6), (34, 37), (19, 12), (21, 48), (3, 18), (27, 2), (40, 49), (1, 17), (41, 11), (33, 12), (13, 25), (18, 4), (42, 14), (20, 34), (2, 4), (13, 26), (45, 30)]</t>
+        </is>
+      </c>
+      <c r="AN29" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>28</v>
+      </c>
+      <c r="C30" t="n">
+        <v>28</v>
+      </c>
+      <c r="D30" t="n">
+        <v>28</v>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr"/>
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="n">
+        <v>519</v>
+      </c>
+      <c r="AJ30" t="inlineStr">
+        <is>
+          <t>['horizontal', 'diagonal', 'horizontal', 'diagonal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'vertical', 'horizontal', 'horizontal', 'vertical', 'vertical', 'horizontal', 'vertical', 'diagonal', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'vertical', 'vertical']</t>
+        </is>
+      </c>
+      <c r="AK30" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL30" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM30" t="inlineStr">
+        <is>
+          <t>[(44, 45), (14, 50), (1, 17), (33, 12), (35, 6), (34, 37), (42, 14), (27, 2), (40, 49), (5, 9), (36, 7), (13, 25), (20, 34), (46, 19), (41, 11), (2, 4), (49, 48), (19, 12), (1, 22), (13, 26), (5, 41), (10, 6), (26, 25), (18, 4), (8, 29), (3, 18), (28, 23), (21, 48), (34, 5), (45, 35), (16, 43), (45, 30), (21, 30), (26, 50), (48, 6)]</t>
+        </is>
+      </c>
+      <c r="AN30" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>29</v>
+      </c>
+      <c r="C31" t="n">
+        <v>29</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr"/>
+      <c r="AI31" t="n">
+        <v>513</v>
+      </c>
+      <c r="AJ31" t="inlineStr">
+        <is>
+          <t>['horizontal', 'diagonal', 'diagonal', 'horizontal', 'vertical', 'diagonal', 'diagonal', 'vertical', 'horizontal', 'vertical', 'vertical', 'vertical', 'vertical', 'diagonal', 'vertical', 'vertical', 'diagonal', 'vertical', 'diagonal', 'horizontal', 'diagonal', 'horizontal', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'horizontal', 'horizontal', 'diagonal', 'diagonal', 'vertical', 'horizontal']</t>
+        </is>
+      </c>
+      <c r="AK31" t="n">
+        <v>366</v>
+      </c>
+      <c r="AL31" t="inlineStr">
+        <is>
+          <t>netlist_5</t>
+        </is>
+      </c>
+      <c r="AM31" t="inlineStr">
+        <is>
+          <t>[(49, 48), (33, 12), (3, 18), (28, 23), (46, 19), (34, 5), (41, 11), (10, 6), (26, 25), (48, 6), (27, 2), (26, 50), (5, 41), (40, 49), (18, 4), (21, 48), (45, 30), (21, 30), (14, 50), (34, 37), (8, 29), (44, 45), (2, 4), (13, 25), (42, 14), (1, 22), (1, 17), (19, 12), (35, 6), (13, 26), (5, 9), (36, 7), (16, 43), (20, 34), (45, 35)]</t>
+        </is>
+      </c>
+      <c r="AN31" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr"/>
+      <c r="AI32" t="n">
+        <v>732</v>
+      </c>
+      <c r="AJ32" t="inlineStr">
+        <is>
+          <t>['diagonal', 'horizontal', 'horizontal', 'horizontal', 'diagonal', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'vertical', 'horizontal', 'horizontal', 'diagonal', 'diagonal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'vertical', 'vertical', 'horizontal', 'vertical', 'horizontal', 'horizontal', 'diagonal', 'horizontal', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'vertical', 'vertical', 'horizontal', 'vertical', 'diagonal', 'vertical', 'diagonal', 'diagonal']</t>
+        </is>
+      </c>
+      <c r="AK32" t="n">
+        <v>472</v>
+      </c>
+      <c r="AL32" t="inlineStr">
+        <is>
+          <t>netlist_6</t>
+        </is>
+      </c>
+      <c r="AM32" t="inlineStr">
+        <is>
+          <t>[(50, 13), (33, 26), (40, 39), (9, 5), (22, 34), (45, 35), (4, 11), (31, 33), (23, 45), (19, 43), (27, 42), (2, 38), (13, 6), (31, 8), (30, 38), (7, 34), (27, 40), (14, 46), (47, 1), (31, 41), (26, 7), (40, 4), (34, 32), (49, 35), (1, 4), (17, 9), (34, 8), (38, 41), (41, 48), (22, 43), (44, 32), (15, 35), (49, 3), (38, 44), (18, 36), (6, 40), (39, 8), (38, 3), (1, 40), (2, 14)]</t>
+        </is>
+      </c>
+      <c r="AN32" t="n">
+        <v>14112</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
+      <c r="AH33" t="inlineStr"/>
+      <c r="AI33" t="n">
+        <v>718</v>
+      </c>
+      <c r="AJ33" t="inlineStr">
+        <is>
+          <t>['diagonal', 'horizontal', 'vertical', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'diagonal', 'diagonal', 'horizontal', 'horizontal', 'vertical', 'vertical', 'diagonal', 'horizontal', 'horizontal', 'horizontal', 'diagonal', 'vertical', 'diagonal', 'diagonal', 'diagonal', 'diagonal', 'vertical', 'diagonal', 'vertical', 'vertical', 'vertical', 'horizontal', 'horizontal', 'horizontal', 'vertical', 'horizontal', 'horizontal']</t>
+        </is>
+      </c>
+      <c r="AK33" t="n">
+        <v>472</v>
+      </c>
+      <c r="AL33" t="inlineStr">
+        <is>
+          <t>netlist_6</t>
+        </is>
+      </c>
+      <c r="AM33" t="inlineStr">
+        <is>
+          <t>[(22, 34), (34, 32), (14, 46), (17, 9), (34, 8), (38, 3), (15, 35), (31, 41), (44, 32), (40, 39), (19, 43), (47, 1), (7, 34), (23, 45), (2, 14), (1, 4), (9, 5), (40, 4), (2, 38), (27, 42), (18, 36), (31, 33), (27, 40), (50, 13), (6, 40), (39, 8), (1, 40), (30, 38), (41, 48), (26, 7), (22, 43), (49, 3), (4, 11), (38, 44), (13, 6), (33, 26), (31, 8), (49, 35), (38, 41), (45, 35)]</t>
+        </is>
+      </c>
+      <c r="AN33" t="n">
         <v>14112</v>
       </c>
     </row>

</xml_diff>